<commit_message>
Working on under ice
</commit_message>
<xml_diff>
--- a/metadata/excel/projects/envonautics/under_ice/metadata.xlsx
+++ b/metadata/excel/projects/envonautics/under_ice/metadata.xlsx
@@ -9,17 +9,17 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-80" yWindow="460" windowWidth="26660" windowHeight="17540" tabRatio="500"/>
+    <workbookView xWindow="80" yWindow="460" windowWidth="26660" windowHeight="17540" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="micans_v6_ex1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="150001" concurrentCalc="0"/>
   <customWorkbookViews>
+    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
+    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
     <customWorkbookView name="Microsoft Office User - Personal View" guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="Me - Personal View" guid="{22DA4066-82A0-D143-AA10-416CFBE3149D}" mergeInterval="0" personalView="1" xWindow="46" yWindow="23" windowWidth="1436" windowHeight="854" tabRatio="500" activeSheetId="1" showStatusbar="0"/>
-    <customWorkbookView name="Kemal - Personal View" guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" mergeInterval="0" personalView="1" xWindow="184" yWindow="84" windowWidth="1280" windowHeight="749" tabRatio="500" activeSheetId="1"/>
-    <customWorkbookView name="LS - Personal View" guid="{06B92370-743D-804F-912C-658BE37B1274}" mergeInterval="0" personalView="1" maximized="1" windowWidth="2556" windowHeight="1244" tabRatio="500" activeSheetId="1"/>
   </customWorkbookViews>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1663" uniqueCount="325">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1782" uniqueCount="403">
   <si>
     <t>Country</t>
   </si>
@@ -1099,6 +1099,240 @@
   </si>
   <si>
     <t>Lake near Krokom</t>
+  </si>
+  <si>
+    <t>20dae0ce479ab7855f5c1db98212d381</t>
+  </si>
+  <si>
+    <t>1696ed7a35473613ce8c193e292926f6</t>
+  </si>
+  <si>
+    <t>155c1e347262fbcfd9481ea010e341ee</t>
+  </si>
+  <si>
+    <t>e6ea5456617a437da15905fe0ffc75aa</t>
+  </si>
+  <si>
+    <t>afecdb71e903bcb78655a54049faccd2</t>
+  </si>
+  <si>
+    <t>8d3047812ac577e463d24f2ee8d03af7</t>
+  </si>
+  <si>
+    <t>7de232541f6613e1951f70a589dadd5c</t>
+  </si>
+  <si>
+    <t>244054a2904d5754b5cf8414618becf1</t>
+  </si>
+  <si>
+    <t>15f326c2220c4946aab7a18e27a2ab23</t>
+  </si>
+  <si>
+    <t>9a658f3cb9a300ebe9ce3898d2c8b16b</t>
+  </si>
+  <si>
+    <t>c58bbd1c6a5c4d342e92b3472e6fb5e4</t>
+  </si>
+  <si>
+    <t>bfec7055123b4c1ca77889c3c62d4359</t>
+  </si>
+  <si>
+    <t>be527d17da3e13b2c2b6fa29f02edb13</t>
+  </si>
+  <si>
+    <t>e8a286b8df7d6aca34332757afad1af8</t>
+  </si>
+  <si>
+    <t>1eac730b744fd1c2f244b6f2b14c3378</t>
+  </si>
+  <si>
+    <t>76d65d56d3ad7f54502488c8246d42e8</t>
+  </si>
+  <si>
+    <t>06604a0cf6b9d09f7b1abdc5b83ed97c</t>
+  </si>
+  <si>
+    <t>7e5df2bdd5b11fe66e82ee50d4583be4</t>
+  </si>
+  <si>
+    <t>85f2614c0e95a71c61ee7a647200161c</t>
+  </si>
+  <si>
+    <t>804d256c66467b965ef19bcd9bf450cd</t>
+  </si>
+  <si>
+    <t>df216b8d53a17f8cd3ba9b6cd3986a12</t>
+  </si>
+  <si>
+    <t>683ed425149b771fd246ceb1a4d2bd15</t>
+  </si>
+  <si>
+    <t>27895ac3dbcf6e77463f0d38b2e9a469</t>
+  </si>
+  <si>
+    <t>f9682aea194452a606b97e8a2cba3607</t>
+  </si>
+  <si>
+    <t>a4e28789de1b9adf3726e4edea532f94</t>
+  </si>
+  <si>
+    <t>2d58292baf58ffc00bffb406570fee37</t>
+  </si>
+  <si>
+    <t>02662af309024e37ed75e29e8748c720</t>
+  </si>
+  <si>
+    <t>8ae6a329673ca7f118ec73c38ddeaf97</t>
+  </si>
+  <si>
+    <t>fbf2a4be1a9777bb2628ac1ef70b01e8</t>
+  </si>
+  <si>
+    <t>604dc1837ab84e429fb14867bc15ca3e</t>
+  </si>
+  <si>
+    <t>5d1406dabfc3b1f296068213378bbdcb</t>
+  </si>
+  <si>
+    <t>cb55a5a8dc01dedc9f43e23248e98e58</t>
+  </si>
+  <si>
+    <t>814512e49361c015ae41c299bbbcfe7f</t>
+  </si>
+  <si>
+    <t>c1c8575a459eefe9ac40c30930700097</t>
+  </si>
+  <si>
+    <t>d8ec9e977d63f12b7147ba2935117230</t>
+  </si>
+  <si>
+    <t>32d1e099f583529fa9fe737f2b03011f</t>
+  </si>
+  <si>
+    <t>d043775d3c82a2ce66b8ae9dfbf460b5</t>
+  </si>
+  <si>
+    <t>58522759d0d75338eccdcbd28c3b75fa</t>
+  </si>
+  <si>
+    <t>f377c02f8f4d4192434c77ba7e626ac4</t>
+  </si>
+  <si>
+    <t>b4cb1a7b3ff03feb309ac1e1ac1bc0cd</t>
+  </si>
+  <si>
+    <t>f9fa6dd67cdc46eaefb0d7ad258c9d4f</t>
+  </si>
+  <si>
+    <t>6333dab67d48a55817e43e29f92b8487</t>
+  </si>
+  <si>
+    <t>96d284d443fd422e00786e8cf0d98ada</t>
+  </si>
+  <si>
+    <t>930f3cc4e8b41d8a67afaa636417a53d</t>
+  </si>
+  <si>
+    <t>6a6ff085bac5c5277c4a2ba1ae0e98e0</t>
+  </si>
+  <si>
+    <t>b57d44b0db588e60aa1eab998c9a5bc8</t>
+  </si>
+  <si>
+    <t>2401cd98f9bead259f8f457192a95e6e</t>
+  </si>
+  <si>
+    <t>008255932a03de707546627e5201f981</t>
+  </si>
+  <si>
+    <t>388091daf4cad9eb2dc06d9a03538260</t>
+  </si>
+  <si>
+    <t>b70c7b95f5a0d399f90535bf077f820a</t>
+  </si>
+  <si>
+    <t>02e33692c57b5cd9a08f041b2458aca1</t>
+  </si>
+  <si>
+    <t>bc864e8a97a12c0a51a11bbfac864836</t>
+  </si>
+  <si>
+    <t>78e30a727d48890f55dc5f04ba914478</t>
+  </si>
+  <si>
+    <t>b73485d2761b019bca3da0de7caf8ac6</t>
+  </si>
+  <si>
+    <t>f0ef4d05aea7079a52d704af0798d05b</t>
+  </si>
+  <si>
+    <t>9ab9132b9d091e6a61f4bab507b31e24</t>
+  </si>
+  <si>
+    <t>3f8112aea2703e6f54633300c729a99c</t>
+  </si>
+  <si>
+    <t>7c98e288a484e1d98be973aaec7caa21</t>
+  </si>
+  <si>
+    <t>d18fd38be02e2c87b71c39e699595b31</t>
+  </si>
+  <si>
+    <t>4a52eef4441fdce8baac2e15573a90e7</t>
+  </si>
+  <si>
+    <t>95afb56ab9c09973dade37bdf78edd48</t>
+  </si>
+  <si>
+    <t>706e2ef652898b983a066a5ecd638bcc</t>
+  </si>
+  <si>
+    <t>9957433bc334c6d416995e786ef93011</t>
+  </si>
+  <si>
+    <t>8547213cc968a8718633abc1c08cde06</t>
+  </si>
+  <si>
+    <t>5949f38d3eefff71bbc1b42ed24e5422</t>
+  </si>
+  <si>
+    <t>412d13dbf2dfc2151b15b13980cd16e0</t>
+  </si>
+  <si>
+    <t>3032f0d88e801d08b87762b91b61f8df</t>
+  </si>
+  <si>
+    <t>a35ea16ee2fa3c3bfd4e86ea3547a75e</t>
+  </si>
+  <si>
+    <t>833e8c774e2ffa0a8f14b09438b85710</t>
+  </si>
+  <si>
+    <t>41930982a1d54fe2e0d32f637cc55f58</t>
+  </si>
+  <si>
+    <t>7b0385bfe733158a1c03ceca8b8920ea</t>
+  </si>
+  <si>
+    <t>28d567b0743b6f5744eb0cb268653da5</t>
+  </si>
+  <si>
+    <t>2bb7b260f942c0efcb9c1fb48795eebc</t>
+  </si>
+  <si>
+    <t>029abb1f2857500032adb9703f456acb</t>
+  </si>
+  <si>
+    <t>4041d0da5d1999106601035f4e50de20</t>
+  </si>
+  <si>
+    <t>08360be1a37ba70cdc07faf56e68b3ae</t>
+  </si>
+  <si>
+    <t>a9771e2f20fc2be558fbca5ea4c2d901</t>
+  </si>
+  <si>
+    <t>158d01406bcf77e8d5e0e35067e6f427</t>
   </si>
 </sst>
 </file>
@@ -1620,7 +1854,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1753,15 +1987,16 @@
     <xf numFmtId="11" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="290"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="291">
     <cellStyle name="Excel Built-in Normal" xfId="267"/>
@@ -2447,10 +2682,10 @@
   </sheetPr>
   <dimension ref="A1:BY64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BC1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="107" zoomScaleNormal="107" zoomScalePageLayoutView="107" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozenSplit"/>
       <selection activeCell="X1" sqref="X1"/>
-      <selection pane="bottomLeft" activeCell="BL16" sqref="BL16"/>
+      <selection pane="bottomLeft" activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2580,24 +2815,24 @@
       <c r="AX1" s="5"/>
       <c r="AY1" s="5"/>
       <c r="AZ1" s="12"/>
-      <c r="BB1" s="62" t="s">
+      <c r="BB1" s="66" t="s">
         <v>32</v>
       </c>
-      <c r="BC1" s="62"/>
-      <c r="BD1" s="62"/>
-      <c r="BE1" s="62"/>
-      <c r="BG1" s="62" t="s">
+      <c r="BC1" s="66"/>
+      <c r="BD1" s="66"/>
+      <c r="BE1" s="66"/>
+      <c r="BG1" s="66" t="s">
         <v>52</v>
       </c>
-      <c r="BH1" s="62"/>
-      <c r="BI1" s="62"/>
-      <c r="BJ1" s="62"/>
-      <c r="BK1" s="62"/>
-      <c r="BL1" s="62"/>
-      <c r="BN1" s="62" t="s">
+      <c r="BH1" s="66"/>
+      <c r="BI1" s="66"/>
+      <c r="BJ1" s="66"/>
+      <c r="BK1" s="66"/>
+      <c r="BL1" s="66"/>
+      <c r="BN1" s="66" t="s">
         <v>66</v>
       </c>
-      <c r="BO1" s="62"/>
+      <c r="BO1" s="66"/>
       <c r="BQ1" s="10" t="s">
         <v>68</v>
       </c>
@@ -2820,7 +3055,7 @@
     </row>
     <row r="3" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A3" s="14">
-        <f>COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BL3,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" ref="A3:A34" si="0">COUNTIF(D3,"&lt;&gt;"&amp;"")+COUNTIF(BL3,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
       </c>
       <c r="B3" s="26">
@@ -2856,10 +3091,21 @@
       <c r="M3" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N3" s="43"/>
-      <c r="O3" s="46"/>
-      <c r="P3" s="60"/>
-      <c r="Q3" s="22"/>
+      <c r="N3" s="43">
+        <v>81389</v>
+      </c>
+      <c r="O3" s="46">
+        <v>81389</v>
+      </c>
+      <c r="P3" s="60" t="s">
+        <v>364</v>
+      </c>
+      <c r="Q3" s="22" t="s">
+        <v>325</v>
+      </c>
+      <c r="R3" t="s">
+        <v>49</v>
+      </c>
       <c r="S3" s="19" t="s">
         <v>267</v>
       </c>
@@ -2873,7 +3119,7 @@
       <c r="W3" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X3" s="64" t="s">
+      <c r="X3" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y3" s="39" t="s">
@@ -2882,27 +3128,27 @@
       <c r="Z3" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA3" s="64" t="s">
+      <c r="AA3" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB3" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC3" s="63" t="s">
+      <c r="AC3" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD3" s="63" t="s">
+      <c r="AD3" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE3" s="63" t="s">
+      <c r="AE3" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="AF3" s="63" t="s">
+      <c r="AF3" s="62" t="s">
         <v>239</v>
       </c>
       <c r="AG3" s="18"/>
       <c r="AH3" s="4"/>
-      <c r="AI3" s="63">
+      <c r="AI3" s="62">
         <v>2.7923583918535537</v>
       </c>
       <c r="AJ3" s="15"/>
@@ -2951,16 +3197,16 @@
       <c r="AZ3">
         <v>300</v>
       </c>
-      <c r="BB3" s="65" t="s">
+      <c r="BB3" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC3" s="65" t="s">
+      <c r="BC3" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD3" s="65" t="s">
+      <c r="BD3" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE3" s="65" t="s">
+      <c r="BE3" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG3" s="28">
@@ -2994,7 +3240,7 @@
     </row>
     <row r="4" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A4" s="14">
-        <f>COUNTIF(D4,"&lt;&gt;"&amp;"")+COUNTIF(BL4,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B4" s="26">
@@ -3030,10 +3276,21 @@
       <c r="M4" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N4" s="43"/>
-      <c r="O4" s="46"/>
-      <c r="P4" s="60"/>
-      <c r="Q4" s="22"/>
+      <c r="N4" s="43">
+        <v>168107</v>
+      </c>
+      <c r="O4" s="46">
+        <v>168107</v>
+      </c>
+      <c r="P4" s="60" t="s">
+        <v>365</v>
+      </c>
+      <c r="Q4" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="R4" t="s">
+        <v>49</v>
+      </c>
       <c r="S4" s="19" t="s">
         <v>268</v>
       </c>
@@ -3047,7 +3304,7 @@
       <c r="W4" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X4" s="64" t="s">
+      <c r="X4" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y4" s="39" t="s">
@@ -3056,27 +3313,27 @@
       <c r="Z4" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA4" s="64" t="s">
+      <c r="AA4" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB4" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC4" s="63" t="s">
+      <c r="AC4" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD4" s="63" t="s">
+      <c r="AD4" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE4" s="63" t="s">
+      <c r="AE4" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="AF4" s="63" t="s">
+      <c r="AF4" s="62" t="s">
         <v>240</v>
       </c>
       <c r="AG4" s="18"/>
       <c r="AH4" s="4"/>
-      <c r="AI4" s="63">
+      <c r="AI4" s="62">
         <v>6.9696773567198482</v>
       </c>
       <c r="AJ4" s="15"/>
@@ -3125,16 +3382,16 @@
       <c r="AZ4">
         <v>300</v>
       </c>
-      <c r="BB4" s="65" t="s">
+      <c r="BB4" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC4" s="65" t="s">
+      <c r="BC4" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD4" s="65" t="s">
+      <c r="BD4" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE4" s="65" t="s">
+      <c r="BE4" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG4" s="28">
@@ -3168,7 +3425,7 @@
     </row>
     <row r="5" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A5" s="14">
-        <f>COUNTIF(D5,"&lt;&gt;"&amp;"")+COUNTIF(BL5,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B5" s="26">
@@ -3204,10 +3461,21 @@
       <c r="M5" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N5" s="43"/>
-      <c r="O5" s="46"/>
-      <c r="P5" s="60"/>
-      <c r="Q5" s="27"/>
+      <c r="N5" s="43">
+        <v>65877</v>
+      </c>
+      <c r="O5" s="46">
+        <v>65877</v>
+      </c>
+      <c r="P5" s="60" t="s">
+        <v>366</v>
+      </c>
+      <c r="Q5" s="27" t="s">
+        <v>327</v>
+      </c>
+      <c r="R5" t="s">
+        <v>49</v>
+      </c>
       <c r="S5" s="19" t="s">
         <v>269</v>
       </c>
@@ -3221,7 +3489,7 @@
       <c r="W5" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X5" s="64" t="s">
+      <c r="X5" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y5" s="39" t="s">
@@ -3230,22 +3498,22 @@
       <c r="Z5" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA5" s="64" t="s">
+      <c r="AA5" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB5" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC5" s="63" t="s">
+      <c r="AC5" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD5" s="63" t="s">
+      <c r="AD5" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE5" s="63" t="s">
+      <c r="AE5" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="AF5" s="63" t="s">
+      <c r="AF5" s="62" t="s">
         <v>241</v>
       </c>
       <c r="AG5" s="18"/>
@@ -3299,16 +3567,16 @@
       <c r="AZ5">
         <v>300</v>
       </c>
-      <c r="BB5" s="65" t="s">
+      <c r="BB5" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC5" s="65" t="s">
+      <c r="BC5" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD5" s="65" t="s">
+      <c r="BD5" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE5" s="65" t="s">
+      <c r="BE5" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG5" s="28">
@@ -3342,7 +3610,7 @@
     </row>
     <row r="6" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A6" s="14">
-        <f>COUNTIF(D6,"&lt;&gt;"&amp;"")+COUNTIF(BL6,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B6" s="26">
@@ -3378,10 +3646,21 @@
       <c r="M6" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N6" s="43"/>
-      <c r="O6" s="46"/>
-      <c r="P6" s="61"/>
-      <c r="Q6" s="22"/>
+      <c r="N6" s="43">
+        <v>119455</v>
+      </c>
+      <c r="O6" s="46">
+        <v>119455</v>
+      </c>
+      <c r="P6" s="61" t="s">
+        <v>367</v>
+      </c>
+      <c r="Q6" s="22" t="s">
+        <v>328</v>
+      </c>
+      <c r="R6" t="s">
+        <v>49</v>
+      </c>
       <c r="S6" s="19" t="s">
         <v>270</v>
       </c>
@@ -3395,7 +3674,7 @@
       <c r="W6" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X6" s="64" t="s">
+      <c r="X6" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y6" s="39" t="s">
@@ -3404,27 +3683,27 @@
       <c r="Z6" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA6" s="64" t="s">
+      <c r="AA6" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB6" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC6" s="63" t="s">
+      <c r="AC6" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD6" s="63" t="s">
+      <c r="AD6" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE6" s="63" t="s">
+      <c r="AE6" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="AF6" s="63" t="s">
+      <c r="AF6" s="62" t="s">
         <v>242</v>
       </c>
       <c r="AG6" s="18"/>
       <c r="AH6" s="4"/>
-      <c r="AI6" s="63">
+      <c r="AI6" s="62">
         <v>11.914501148830135</v>
       </c>
       <c r="AJ6" s="15"/>
@@ -3473,16 +3752,16 @@
       <c r="AZ6">
         <v>300</v>
       </c>
-      <c r="BB6" s="65" t="s">
+      <c r="BB6" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC6" s="65" t="s">
+      <c r="BC6" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD6" s="65" t="s">
+      <c r="BD6" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE6" s="65" t="s">
+      <c r="BE6" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG6" s="28">
@@ -3516,7 +3795,7 @@
     </row>
     <row r="7" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A7" s="14">
-        <f>COUNTIF(D7,"&lt;&gt;"&amp;"")+COUNTIF(BL7,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B7" s="26">
@@ -3552,10 +3831,21 @@
       <c r="M7" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N7" s="43"/>
-      <c r="O7" s="46"/>
-      <c r="P7" s="60"/>
-      <c r="Q7" s="22"/>
+      <c r="N7" s="43">
+        <v>89396</v>
+      </c>
+      <c r="O7" s="46">
+        <v>89396</v>
+      </c>
+      <c r="P7" s="60" t="s">
+        <v>368</v>
+      </c>
+      <c r="Q7" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="R7" t="s">
+        <v>49</v>
+      </c>
       <c r="S7" s="19" t="s">
         <v>271</v>
       </c>
@@ -3569,7 +3859,7 @@
       <c r="W7" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X7" s="64" t="s">
+      <c r="X7" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y7" s="39" t="s">
@@ -3578,27 +3868,27 @@
       <c r="Z7" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA7" s="64" t="s">
+      <c r="AA7" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC7" s="63" t="s">
+      <c r="AC7" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD7" s="63" t="s">
+      <c r="AD7" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE7" s="63" t="s">
+      <c r="AE7" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="AF7" s="63" t="s">
+      <c r="AF7" s="62" t="s">
         <v>243</v>
       </c>
       <c r="AG7" s="18"/>
       <c r="AH7" s="4"/>
-      <c r="AI7" s="63">
+      <c r="AI7" s="62">
         <v>9.4447860371293277</v>
       </c>
       <c r="AJ7" s="15"/>
@@ -3647,16 +3937,16 @@
       <c r="AZ7">
         <v>300</v>
       </c>
-      <c r="BB7" s="65" t="s">
+      <c r="BB7" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC7" s="65" t="s">
+      <c r="BC7" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD7" s="65" t="s">
+      <c r="BD7" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE7" s="65" t="s">
+      <c r="BE7" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG7" s="28">
@@ -3690,7 +3980,7 @@
     </row>
     <row r="8" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A8" s="14">
-        <f>COUNTIF(D8,"&lt;&gt;"&amp;"")+COUNTIF(BL8,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B8" s="26">
@@ -3726,10 +4016,21 @@
       <c r="M8" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N8" s="43"/>
-      <c r="O8" s="46"/>
-      <c r="P8" s="60"/>
-      <c r="Q8" s="27"/>
+      <c r="N8" s="43">
+        <v>226665</v>
+      </c>
+      <c r="O8" s="46">
+        <v>226665</v>
+      </c>
+      <c r="P8" s="60" t="s">
+        <v>369</v>
+      </c>
+      <c r="Q8" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="R8" t="s">
+        <v>49</v>
+      </c>
       <c r="S8" s="19" t="s">
         <v>272</v>
       </c>
@@ -3743,7 +4044,7 @@
       <c r="W8" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X8" s="64" t="s">
+      <c r="X8" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y8" s="39" t="s">
@@ -3752,27 +4053,27 @@
       <c r="Z8" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA8" s="64" t="s">
+      <c r="AA8" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB8" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC8" s="63" t="s">
+      <c r="AC8" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD8" s="63" t="s">
+      <c r="AD8" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE8" s="63" t="s">
+      <c r="AE8" s="62" t="s">
         <v>260</v>
       </c>
-      <c r="AF8" s="63" t="s">
+      <c r="AF8" s="62" t="s">
         <v>244</v>
       </c>
       <c r="AG8" s="18"/>
       <c r="AH8" s="4"/>
-      <c r="AI8" s="63">
+      <c r="AI8" s="62">
         <v>16.652751259398293</v>
       </c>
       <c r="AJ8" s="15"/>
@@ -3821,16 +4122,16 @@
       <c r="AZ8">
         <v>300</v>
       </c>
-      <c r="BB8" s="65" t="s">
+      <c r="BB8" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC8" s="65" t="s">
+      <c r="BC8" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD8" s="65" t="s">
+      <c r="BD8" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE8" s="65" t="s">
+      <c r="BE8" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG8" s="28">
@@ -3864,7 +4165,7 @@
     </row>
     <row r="9" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A9" s="14">
-        <f>COUNTIF(D9,"&lt;&gt;"&amp;"")+COUNTIF(BL9,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B9" s="26">
@@ -3900,10 +4201,21 @@
       <c r="M9" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N9" s="43"/>
-      <c r="O9" s="46"/>
-      <c r="P9" s="60"/>
-      <c r="Q9" s="22"/>
+      <c r="N9" s="43">
+        <v>160204</v>
+      </c>
+      <c r="O9" s="46">
+        <v>160204</v>
+      </c>
+      <c r="P9" s="60" t="s">
+        <v>370</v>
+      </c>
+      <c r="Q9" s="22" t="s">
+        <v>331</v>
+      </c>
+      <c r="R9" t="s">
+        <v>49</v>
+      </c>
       <c r="S9" s="19" t="s">
         <v>273</v>
       </c>
@@ -3917,7 +4229,7 @@
       <c r="W9" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X9" s="64" t="s">
+      <c r="X9" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y9" s="39" t="s">
@@ -3926,27 +4238,27 @@
       <c r="Z9" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA9" s="64" t="s">
+      <c r="AA9" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC9" s="63" t="s">
+      <c r="AC9" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD9" s="63" t="s">
+      <c r="AD9" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE9" s="63" t="s">
+      <c r="AE9" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="AF9" s="63" t="s">
+      <c r="AF9" s="62" t="s">
         <v>245</v>
       </c>
       <c r="AG9" s="18"/>
       <c r="AH9" s="4"/>
-      <c r="AI9" s="63">
+      <c r="AI9" s="62">
         <v>16.168408789359567</v>
       </c>
       <c r="AJ9" s="15"/>
@@ -3995,16 +4307,16 @@
       <c r="AZ9">
         <v>300</v>
       </c>
-      <c r="BB9" s="65" t="s">
+      <c r="BB9" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC9" s="65" t="s">
+      <c r="BC9" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD9" s="65" t="s">
+      <c r="BD9" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE9" s="65" t="s">
+      <c r="BE9" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG9" s="28">
@@ -4038,7 +4350,7 @@
     </row>
     <row r="10" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A10" s="14">
-        <f>COUNTIF(D10,"&lt;&gt;"&amp;"")+COUNTIF(BL10,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B10" s="26">
@@ -4074,10 +4386,21 @@
       <c r="M10" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N10" s="43"/>
-      <c r="O10" s="46"/>
-      <c r="P10" s="60"/>
-      <c r="Q10" s="22"/>
+      <c r="N10" s="43">
+        <v>164342</v>
+      </c>
+      <c r="O10" s="46">
+        <v>164342</v>
+      </c>
+      <c r="P10" s="60" t="s">
+        <v>371</v>
+      </c>
+      <c r="Q10" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="R10" t="s">
+        <v>49</v>
+      </c>
       <c r="S10" s="19" t="s">
         <v>274</v>
       </c>
@@ -4091,7 +4414,7 @@
       <c r="W10" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X10" s="64" t="s">
+      <c r="X10" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y10" s="39" t="s">
@@ -4100,27 +4423,27 @@
       <c r="Z10" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA10" s="64" t="s">
+      <c r="AA10" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB10" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC10" s="63" t="s">
+      <c r="AC10" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD10" s="63" t="s">
+      <c r="AD10" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE10" s="63" t="s">
+      <c r="AE10" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="AF10" s="63" t="s">
+      <c r="AF10" s="62" t="s">
         <v>246</v>
       </c>
       <c r="AG10" s="18"/>
       <c r="AH10" s="4"/>
-      <c r="AI10" s="63">
+      <c r="AI10" s="62">
         <v>4.8327454343440888</v>
       </c>
       <c r="AJ10" s="15"/>
@@ -4169,16 +4492,16 @@
       <c r="AZ10">
         <v>300</v>
       </c>
-      <c r="BB10" s="65" t="s">
+      <c r="BB10" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC10" s="65" t="s">
+      <c r="BC10" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD10" s="65" t="s">
+      <c r="BD10" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE10" s="65" t="s">
+      <c r="BE10" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG10" s="28">
@@ -4212,7 +4535,7 @@
     </row>
     <row r="11" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A11" s="14">
-        <f>COUNTIF(D11,"&lt;&gt;"&amp;"")+COUNTIF(BL11,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B11" s="26">
@@ -4248,10 +4571,21 @@
       <c r="M11" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N11" s="43"/>
-      <c r="O11" s="46"/>
-      <c r="P11" s="60"/>
-      <c r="Q11" s="22"/>
+      <c r="N11" s="43">
+        <v>180781</v>
+      </c>
+      <c r="O11" s="46">
+        <v>180781</v>
+      </c>
+      <c r="P11" s="60" t="s">
+        <v>372</v>
+      </c>
+      <c r="Q11" s="22" t="s">
+        <v>333</v>
+      </c>
+      <c r="R11" t="s">
+        <v>49</v>
+      </c>
       <c r="S11" s="19" t="s">
         <v>275</v>
       </c>
@@ -4265,7 +4599,7 @@
       <c r="W11" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X11" s="64" t="s">
+      <c r="X11" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y11" s="39" t="s">
@@ -4274,27 +4608,27 @@
       <c r="Z11" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA11" s="64" t="s">
+      <c r="AA11" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB11" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC11" s="63" t="s">
+      <c r="AC11" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD11" s="63" t="s">
+      <c r="AD11" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE11" s="63" t="s">
+      <c r="AE11" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="AF11" s="63" t="s">
+      <c r="AF11" s="62" t="s">
         <v>247</v>
       </c>
       <c r="AG11" s="18"/>
       <c r="AH11" s="4"/>
-      <c r="AI11" s="63">
+      <c r="AI11" s="62">
         <v>28.768324649687713</v>
       </c>
       <c r="AJ11" s="15"/>
@@ -4343,16 +4677,16 @@
       <c r="AZ11">
         <v>300</v>
       </c>
-      <c r="BB11" s="65" t="s">
+      <c r="BB11" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC11" s="65" t="s">
+      <c r="BC11" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD11" s="65" t="s">
+      <c r="BD11" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE11" s="65" t="s">
+      <c r="BE11" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG11" s="28">
@@ -4367,7 +4701,7 @@
       <c r="BJ11" t="s">
         <v>323</v>
       </c>
-      <c r="BK11" s="66" t="s">
+      <c r="BK11" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL11" s="29"/>
@@ -4388,7 +4722,7 @@
     </row>
     <row r="12" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A12" s="14">
-        <f>COUNTIF(D12,"&lt;&gt;"&amp;"")+COUNTIF(BL12,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B12" s="26">
@@ -4424,10 +4758,21 @@
       <c r="M12" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N12" s="43"/>
-      <c r="O12" s="46"/>
-      <c r="P12" s="60"/>
-      <c r="Q12" s="27"/>
+      <c r="N12" s="43">
+        <v>217299</v>
+      </c>
+      <c r="O12" s="46">
+        <v>217299</v>
+      </c>
+      <c r="P12" s="60" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q12" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="R12" t="s">
+        <v>49</v>
+      </c>
       <c r="S12" s="19" t="s">
         <v>276</v>
       </c>
@@ -4441,7 +4786,7 @@
       <c r="W12" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X12" s="64" t="s">
+      <c r="X12" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y12" s="39" t="s">
@@ -4450,27 +4795,27 @@
       <c r="Z12" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA12" s="64" t="s">
+      <c r="AA12" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB12" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC12" s="63" t="s">
+      <c r="AC12" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD12" s="63" t="s">
+      <c r="AD12" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE12" s="63" t="s">
+      <c r="AE12" s="62" t="s">
         <v>264</v>
       </c>
-      <c r="AF12" s="63" t="s">
+      <c r="AF12" s="62" t="s">
         <v>248</v>
       </c>
       <c r="AG12" s="18"/>
       <c r="AH12" s="4"/>
-      <c r="AI12" s="63">
+      <c r="AI12" s="62">
         <v>11.041282374896175</v>
       </c>
       <c r="AJ12" s="15"/>
@@ -4519,16 +4864,16 @@
       <c r="AZ12">
         <v>300</v>
       </c>
-      <c r="BB12" s="65" t="s">
+      <c r="BB12" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC12" s="65" t="s">
+      <c r="BC12" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD12" s="65" t="s">
+      <c r="BD12" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE12" s="65" t="s">
+      <c r="BE12" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG12" s="28">
@@ -4543,7 +4888,7 @@
       <c r="BJ12" t="s">
         <v>323</v>
       </c>
-      <c r="BK12" s="66" t="s">
+      <c r="BK12" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL12" s="29"/>
@@ -4564,7 +4909,7 @@
     </row>
     <row r="13" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A13" s="14">
-        <f>COUNTIF(D13,"&lt;&gt;"&amp;"")+COUNTIF(BL13,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B13" s="26">
@@ -4600,10 +4945,21 @@
       <c r="M13" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N13" s="43"/>
-      <c r="O13" s="46"/>
-      <c r="P13" s="60"/>
-      <c r="Q13" s="22"/>
+      <c r="N13" s="43">
+        <v>171813</v>
+      </c>
+      <c r="O13" s="46">
+        <v>171813</v>
+      </c>
+      <c r="P13" s="60" t="s">
+        <v>374</v>
+      </c>
+      <c r="Q13" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="R13" t="s">
+        <v>49</v>
+      </c>
       <c r="S13" s="19" t="s">
         <v>277</v>
       </c>
@@ -4617,7 +4973,7 @@
       <c r="W13" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X13" s="64" t="s">
+      <c r="X13" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y13" s="39" t="s">
@@ -4626,27 +4982,27 @@
       <c r="Z13" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA13" s="64" t="s">
+      <c r="AA13" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB13" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC13" s="63" t="s">
+      <c r="AC13" s="62" t="s">
         <v>251</v>
       </c>
-      <c r="AD13" s="63" t="s">
+      <c r="AD13" s="62" t="s">
         <v>235</v>
       </c>
-      <c r="AE13" s="63" t="s">
+      <c r="AE13" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="AF13" s="63" t="s">
+      <c r="AF13" s="62" t="s">
         <v>249</v>
       </c>
       <c r="AG13" s="18"/>
       <c r="AH13" s="4"/>
-      <c r="AI13" s="63">
+      <c r="AI13" s="62">
         <v>30.481861428432737</v>
       </c>
       <c r="AJ13" s="15"/>
@@ -4695,16 +5051,16 @@
       <c r="AZ13">
         <v>300</v>
       </c>
-      <c r="BB13" s="65" t="s">
+      <c r="BB13" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC13" s="65" t="s">
+      <c r="BC13" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD13" s="65" t="s">
+      <c r="BD13" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE13" s="65" t="s">
+      <c r="BE13" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG13" s="28">
@@ -4719,7 +5075,7 @@
       <c r="BJ13" t="s">
         <v>323</v>
       </c>
-      <c r="BK13" s="66" t="s">
+      <c r="BK13" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL13" s="29"/>
@@ -4740,7 +5096,7 @@
     </row>
     <row r="14" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A14" s="14">
-        <f>COUNTIF(D14,"&lt;&gt;"&amp;"")+COUNTIF(BL14,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B14" s="26">
@@ -4776,10 +5132,21 @@
       <c r="M14" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N14" s="43"/>
-      <c r="O14" s="46"/>
-      <c r="P14" s="60"/>
-      <c r="Q14" s="22"/>
+      <c r="N14" s="43">
+        <v>167254</v>
+      </c>
+      <c r="O14" s="46">
+        <v>167254</v>
+      </c>
+      <c r="P14" s="61" t="s">
+        <v>375</v>
+      </c>
+      <c r="Q14" s="22" t="s">
+        <v>336</v>
+      </c>
+      <c r="R14" t="s">
+        <v>49</v>
+      </c>
       <c r="S14" s="19" t="s">
         <v>278</v>
       </c>
@@ -4793,7 +5160,7 @@
       <c r="W14" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X14" s="64" t="s">
+      <c r="X14" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y14" s="39" t="s">
@@ -4802,27 +5169,27 @@
       <c r="Z14" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA14" s="64" t="s">
+      <c r="AA14" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB14" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC14" s="63" t="s">
+      <c r="AC14" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD14" s="63" t="s">
+      <c r="AD14" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE14" s="63" t="s">
+      <c r="AE14" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="AF14" s="63" t="s">
+      <c r="AF14" s="62" t="s">
         <v>250</v>
       </c>
       <c r="AG14" s="18"/>
       <c r="AH14" s="4"/>
-      <c r="AI14" s="63">
+      <c r="AI14" s="62">
         <v>9.7737937283583065</v>
       </c>
       <c r="AJ14" s="15"/>
@@ -4871,16 +5238,16 @@
       <c r="AZ14">
         <v>300</v>
       </c>
-      <c r="BB14" s="65" t="s">
+      <c r="BB14" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC14" s="65" t="s">
+      <c r="BC14" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD14" s="65" t="s">
+      <c r="BD14" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE14" s="65" t="s">
+      <c r="BE14" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG14" s="28">
@@ -4895,7 +5262,7 @@
       <c r="BJ14" t="s">
         <v>323</v>
       </c>
-      <c r="BK14" s="66" t="s">
+      <c r="BK14" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL14" s="29"/>
@@ -4916,7 +5283,7 @@
     </row>
     <row r="15" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A15" s="14">
-        <f>COUNTIF(D15,"&lt;&gt;"&amp;"")+COUNTIF(BL15,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B15" s="26">
@@ -4952,10 +5319,21 @@
       <c r="M15" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N15" s="43"/>
-      <c r="O15" s="46"/>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="22"/>
+      <c r="N15" s="43">
+        <v>132653</v>
+      </c>
+      <c r="O15" s="46">
+        <v>132653</v>
+      </c>
+      <c r="P15" s="60" t="s">
+        <v>376</v>
+      </c>
+      <c r="Q15" s="22" t="s">
+        <v>337</v>
+      </c>
+      <c r="R15" t="s">
+        <v>49</v>
+      </c>
       <c r="S15" s="19" t="s">
         <v>279</v>
       </c>
@@ -4969,7 +5347,7 @@
       <c r="W15" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X15" s="64" t="s">
+      <c r="X15" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y15" s="39" t="s">
@@ -4978,27 +5356,27 @@
       <c r="Z15" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA15" s="64" t="s">
+      <c r="AA15" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC15" s="63" t="s">
+      <c r="AC15" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD15" s="63" t="s">
+      <c r="AD15" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE15" s="63" t="s">
+      <c r="AE15" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="AF15" s="63" t="s">
+      <c r="AF15" s="62" t="s">
         <v>239</v>
       </c>
       <c r="AG15" s="18"/>
       <c r="AH15" s="4"/>
-      <c r="AI15" s="63">
+      <c r="AI15" s="62">
         <v>11.207943647994133</v>
       </c>
       <c r="AJ15" s="15"/>
@@ -5047,16 +5425,16 @@
       <c r="AZ15">
         <v>300</v>
       </c>
-      <c r="BB15" s="65" t="s">
+      <c r="BB15" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC15" s="65" t="s">
+      <c r="BC15" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD15" s="65" t="s">
+      <c r="BD15" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE15" s="65" t="s">
+      <c r="BE15" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG15" s="28">
@@ -5071,7 +5449,7 @@
       <c r="BJ15" t="s">
         <v>323</v>
       </c>
-      <c r="BK15" s="66" t="s">
+      <c r="BK15" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL15" s="29"/>
@@ -5092,7 +5470,7 @@
     </row>
     <row r="16" spans="1:77" x14ac:dyDescent="0.2">
       <c r="A16" s="14">
-        <f>COUNTIF(D16,"&lt;&gt;"&amp;"")+COUNTIF(BL16,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B16" s="26">
@@ -5128,10 +5506,21 @@
       <c r="M16" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N16" s="43"/>
-      <c r="O16" s="46"/>
-      <c r="P16" s="60"/>
-      <c r="Q16" s="22"/>
+      <c r="N16" s="43">
+        <v>203523</v>
+      </c>
+      <c r="O16" s="46">
+        <v>203523</v>
+      </c>
+      <c r="P16" s="60" t="s">
+        <v>377</v>
+      </c>
+      <c r="Q16" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="R16" t="s">
+        <v>49</v>
+      </c>
       <c r="S16" s="19" t="s">
         <v>280</v>
       </c>
@@ -5145,7 +5534,7 @@
       <c r="W16" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X16" s="64" t="s">
+      <c r="X16" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y16" s="39" t="s">
@@ -5154,27 +5543,27 @@
       <c r="Z16" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA16" s="64" t="s">
+      <c r="AA16" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB16" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC16" s="63" t="s">
+      <c r="AC16" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD16" s="63" t="s">
+      <c r="AD16" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE16" s="63" t="s">
+      <c r="AE16" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="AF16" s="63" t="s">
+      <c r="AF16" s="62" t="s">
         <v>240</v>
       </c>
       <c r="AG16" s="18"/>
       <c r="AH16" s="4"/>
-      <c r="AI16" s="63">
+      <c r="AI16" s="62">
         <v>11.713860392867545</v>
       </c>
       <c r="AJ16" s="15"/>
@@ -5223,16 +5612,16 @@
       <c r="AZ16">
         <v>300</v>
       </c>
-      <c r="BB16" s="65" t="s">
+      <c r="BB16" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC16" s="65" t="s">
+      <c r="BC16" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD16" s="65" t="s">
+      <c r="BD16" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE16" s="65" t="s">
+      <c r="BE16" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG16" s="28">
@@ -5247,7 +5636,7 @@
       <c r="BJ16" t="s">
         <v>323</v>
       </c>
-      <c r="BK16" s="66" t="s">
+      <c r="BK16" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL16" s="29"/>
@@ -5268,7 +5657,7 @@
     </row>
     <row r="17" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A17" s="14">
-        <f>COUNTIF(D17,"&lt;&gt;"&amp;"")+COUNTIF(BL17,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B17" s="26">
@@ -5304,10 +5693,21 @@
       <c r="M17" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N17" s="43"/>
-      <c r="O17" s="46"/>
-      <c r="P17" s="61"/>
-      <c r="Q17" s="22"/>
+      <c r="N17" s="43">
+        <v>144012</v>
+      </c>
+      <c r="O17" s="46">
+        <v>144012</v>
+      </c>
+      <c r="P17" s="61" t="s">
+        <v>378</v>
+      </c>
+      <c r="Q17" s="22" t="s">
+        <v>339</v>
+      </c>
+      <c r="R17" t="s">
+        <v>49</v>
+      </c>
       <c r="S17" s="19" t="s">
         <v>281</v>
       </c>
@@ -5321,7 +5721,7 @@
       <c r="W17" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X17" s="64" t="s">
+      <c r="X17" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y17" s="39" t="s">
@@ -5330,27 +5730,27 @@
       <c r="Z17" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA17" s="64" t="s">
+      <c r="AA17" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC17" s="63" t="s">
+      <c r="AC17" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD17" s="63" t="s">
+      <c r="AD17" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE17" s="63" t="s">
+      <c r="AE17" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="AF17" s="63" t="s">
+      <c r="AF17" s="62" t="s">
         <v>241</v>
       </c>
       <c r="AG17" s="18"/>
       <c r="AH17" s="4"/>
-      <c r="AI17" s="63">
+      <c r="AI17" s="62">
         <v>6.0511526056330434</v>
       </c>
       <c r="AJ17" s="15"/>
@@ -5399,16 +5799,16 @@
       <c r="AZ17">
         <v>300</v>
       </c>
-      <c r="BB17" s="65" t="s">
+      <c r="BB17" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC17" s="65" t="s">
+      <c r="BC17" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD17" s="65" t="s">
+      <c r="BD17" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE17" s="65" t="s">
+      <c r="BE17" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG17" s="28">
@@ -5423,7 +5823,7 @@
       <c r="BJ17" t="s">
         <v>323</v>
       </c>
-      <c r="BK17" s="66" t="s">
+      <c r="BK17" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL17" s="29"/>
@@ -5444,7 +5844,7 @@
     </row>
     <row r="18" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A18" s="14">
-        <f>COUNTIF(D18,"&lt;&gt;"&amp;"")+COUNTIF(BL18,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B18" s="26">
@@ -5480,10 +5880,21 @@
       <c r="M18" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N18" s="43"/>
-      <c r="O18" s="46"/>
-      <c r="P18" s="60"/>
-      <c r="Q18" s="22"/>
+      <c r="N18" s="43">
+        <v>129352</v>
+      </c>
+      <c r="O18" s="46">
+        <v>129352</v>
+      </c>
+      <c r="P18" s="60" t="s">
+        <v>379</v>
+      </c>
+      <c r="Q18" s="22" t="s">
+        <v>340</v>
+      </c>
+      <c r="R18" t="s">
+        <v>49</v>
+      </c>
       <c r="S18" s="19" t="s">
         <v>282</v>
       </c>
@@ -5497,7 +5908,7 @@
       <c r="W18" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X18" s="64" t="s">
+      <c r="X18" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y18" s="39" t="s">
@@ -5506,27 +5917,27 @@
       <c r="Z18" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA18" s="64" t="s">
+      <c r="AA18" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB18" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC18" s="63" t="s">
+      <c r="AC18" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD18" s="63" t="s">
+      <c r="AD18" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE18" s="63" t="s">
+      <c r="AE18" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="AF18" s="63" t="s">
+      <c r="AF18" s="62" t="s">
         <v>242</v>
       </c>
       <c r="AG18" s="18"/>
       <c r="AH18" s="4"/>
-      <c r="AI18" s="63">
+      <c r="AI18" s="62">
         <v>7.8838872528397141</v>
       </c>
       <c r="AJ18" s="15"/>
@@ -5575,16 +5986,16 @@
       <c r="AZ18">
         <v>300</v>
       </c>
-      <c r="BB18" s="65" t="s">
+      <c r="BB18" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC18" s="65" t="s">
+      <c r="BC18" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD18" s="65" t="s">
+      <c r="BD18" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE18" s="65" t="s">
+      <c r="BE18" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG18" s="28">
@@ -5599,7 +6010,7 @@
       <c r="BJ18" t="s">
         <v>323</v>
       </c>
-      <c r="BK18" s="66" t="s">
+      <c r="BK18" s="65" t="s">
         <v>324</v>
       </c>
       <c r="BL18" s="29"/>
@@ -5620,7 +6031,7 @@
     </row>
     <row r="19" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A19" s="14">
-        <f>COUNTIF(D19,"&lt;&gt;"&amp;"")+COUNTIF(BL19,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B19" s="26">
@@ -5656,10 +6067,21 @@
       <c r="M19" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N19" s="43"/>
-      <c r="O19" s="46"/>
-      <c r="P19" s="60"/>
-      <c r="Q19" s="22"/>
+      <c r="N19" s="43">
+        <v>160967</v>
+      </c>
+      <c r="O19" s="46">
+        <v>160967</v>
+      </c>
+      <c r="P19" s="60" t="s">
+        <v>380</v>
+      </c>
+      <c r="Q19" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="R19" t="s">
+        <v>49</v>
+      </c>
       <c r="S19" s="19" t="s">
         <v>283</v>
       </c>
@@ -5673,7 +6095,7 @@
       <c r="W19" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X19" s="64" t="s">
+      <c r="X19" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y19" s="39" t="s">
@@ -5682,27 +6104,27 @@
       <c r="Z19" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA19" s="64" t="s">
+      <c r="AA19" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB19" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC19" s="63" t="s">
+      <c r="AC19" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD19" s="63" t="s">
+      <c r="AD19" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE19" s="63" t="s">
+      <c r="AE19" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="AF19" s="63" t="s">
+      <c r="AF19" s="62" t="s">
         <v>243</v>
       </c>
       <c r="AG19" s="18"/>
       <c r="AH19" s="4"/>
-      <c r="AI19" s="63">
+      <c r="AI19" s="62">
         <v>11.490566648328533</v>
       </c>
       <c r="AJ19" s="15"/>
@@ -5751,16 +6173,16 @@
       <c r="AZ19">
         <v>300</v>
       </c>
-      <c r="BB19" s="65" t="s">
+      <c r="BB19" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC19" s="65" t="s">
+      <c r="BC19" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD19" s="65" t="s">
+      <c r="BD19" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE19" s="65" t="s">
+      <c r="BE19" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG19" s="28">
@@ -5794,7 +6216,7 @@
     </row>
     <row r="20" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A20" s="14">
-        <f>COUNTIF(D20,"&lt;&gt;"&amp;"")+COUNTIF(BL20,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B20" s="26">
@@ -5830,10 +6252,21 @@
       <c r="M20" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N20" s="43"/>
-      <c r="O20" s="46"/>
-      <c r="P20" s="60"/>
-      <c r="Q20" s="22"/>
+      <c r="N20" s="43">
+        <v>133420</v>
+      </c>
+      <c r="O20" s="46">
+        <v>133420</v>
+      </c>
+      <c r="P20" s="60" t="s">
+        <v>381</v>
+      </c>
+      <c r="Q20" s="22" t="s">
+        <v>342</v>
+      </c>
+      <c r="R20" t="s">
+        <v>49</v>
+      </c>
       <c r="S20" s="19" t="s">
         <v>284</v>
       </c>
@@ -5847,7 +6280,7 @@
       <c r="W20" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X20" s="64" t="s">
+      <c r="X20" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y20" s="39" t="s">
@@ -5856,27 +6289,27 @@
       <c r="Z20" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA20" s="64" t="s">
+      <c r="AA20" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB20" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC20" s="63" t="s">
+      <c r="AC20" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD20" s="63" t="s">
+      <c r="AD20" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE20" s="63" t="s">
+      <c r="AE20" s="62" t="s">
         <v>260</v>
       </c>
-      <c r="AF20" s="63" t="s">
+      <c r="AF20" s="62" t="s">
         <v>244</v>
       </c>
       <c r="AG20" s="18"/>
       <c r="AH20" s="4"/>
-      <c r="AI20" s="63">
+      <c r="AI20" s="62">
         <v>4.5328630141419373</v>
       </c>
       <c r="AJ20" s="15"/>
@@ -5925,16 +6358,16 @@
       <c r="AZ20">
         <v>300</v>
       </c>
-      <c r="BB20" s="65" t="s">
+      <c r="BB20" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC20" s="65" t="s">
+      <c r="BC20" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD20" s="65" t="s">
+      <c r="BD20" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE20" s="65" t="s">
+      <c r="BE20" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG20" s="28">
@@ -5968,7 +6401,7 @@
     </row>
     <row r="21" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A21" s="14">
-        <f>COUNTIF(D21,"&lt;&gt;"&amp;"")+COUNTIF(BL21,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B21" s="26">
@@ -6004,10 +6437,21 @@
       <c r="M21" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N21" s="43"/>
-      <c r="O21" s="46"/>
-      <c r="P21" s="60"/>
-      <c r="Q21" s="22"/>
+      <c r="N21" s="43">
+        <v>104961</v>
+      </c>
+      <c r="O21" s="46">
+        <v>104961</v>
+      </c>
+      <c r="P21" s="60" t="s">
+        <v>382</v>
+      </c>
+      <c r="Q21" s="22" t="s">
+        <v>343</v>
+      </c>
+      <c r="R21" t="s">
+        <v>49</v>
+      </c>
       <c r="S21" s="19" t="s">
         <v>285</v>
       </c>
@@ -6021,7 +6465,7 @@
       <c r="W21" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X21" s="64" t="s">
+      <c r="X21" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y21" s="39" t="s">
@@ -6030,27 +6474,27 @@
       <c r="Z21" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA21" s="64" t="s">
+      <c r="AA21" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB21" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC21" s="63" t="s">
+      <c r="AC21" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD21" s="63" t="s">
+      <c r="AD21" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE21" s="63" t="s">
+      <c r="AE21" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="AF21" s="63" t="s">
+      <c r="AF21" s="62" t="s">
         <v>245</v>
       </c>
       <c r="AG21" s="18"/>
       <c r="AH21" s="4"/>
-      <c r="AI21" s="63">
+      <c r="AI21" s="62">
         <v>12.054733935255602</v>
       </c>
       <c r="AJ21" s="15"/>
@@ -6099,16 +6543,16 @@
       <c r="AZ21">
         <v>300</v>
       </c>
-      <c r="BB21" s="65" t="s">
+      <c r="BB21" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC21" s="65" t="s">
+      <c r="BC21" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD21" s="65" t="s">
+      <c r="BD21" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE21" s="65" t="s">
+      <c r="BE21" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG21" s="28">
@@ -6142,7 +6586,7 @@
     </row>
     <row r="22" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A22" s="14">
-        <f>COUNTIF(D22,"&lt;&gt;"&amp;"")+COUNTIF(BL22,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B22" s="26">
@@ -6178,10 +6622,21 @@
       <c r="M22" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N22" s="43"/>
-      <c r="O22" s="46"/>
-      <c r="P22" s="60"/>
-      <c r="Q22" s="22"/>
+      <c r="N22" s="43">
+        <v>169176</v>
+      </c>
+      <c r="O22" s="46">
+        <v>169176</v>
+      </c>
+      <c r="P22" s="60" t="s">
+        <v>383</v>
+      </c>
+      <c r="Q22" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="R22" t="s">
+        <v>49</v>
+      </c>
       <c r="S22" s="19" t="s">
         <v>286</v>
       </c>
@@ -6195,7 +6650,7 @@
       <c r="W22" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X22" s="64" t="s">
+      <c r="X22" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y22" s="39" t="s">
@@ -6204,27 +6659,27 @@
       <c r="Z22" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA22" s="64" t="s">
+      <c r="AA22" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB22" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC22" s="63" t="s">
+      <c r="AC22" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD22" s="63" t="s">
+      <c r="AD22" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE22" s="63" t="s">
+      <c r="AE22" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="AF22" s="63" t="s">
+      <c r="AF22" s="62" t="s">
         <v>246</v>
       </c>
       <c r="AG22" s="18"/>
       <c r="AH22" s="4"/>
-      <c r="AI22" s="63">
+      <c r="AI22" s="62">
         <v>1.6402921156812615</v>
       </c>
       <c r="AJ22" s="15"/>
@@ -6273,16 +6728,16 @@
       <c r="AZ22">
         <v>300</v>
       </c>
-      <c r="BB22" s="65" t="s">
+      <c r="BB22" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC22" s="65" t="s">
+      <c r="BC22" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD22" s="65" t="s">
+      <c r="BD22" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE22" s="65" t="s">
+      <c r="BE22" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG22" s="28">
@@ -6316,7 +6771,7 @@
     </row>
     <row r="23" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A23" s="14">
-        <f>COUNTIF(D23,"&lt;&gt;"&amp;"")+COUNTIF(BL23,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B23" s="26">
@@ -6352,10 +6807,21 @@
       <c r="M23" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N23" s="43"/>
-      <c r="O23" s="46"/>
-      <c r="P23" s="60"/>
-      <c r="Q23" s="22"/>
+      <c r="N23" s="43">
+        <v>116053</v>
+      </c>
+      <c r="O23" s="46">
+        <v>116053</v>
+      </c>
+      <c r="P23" s="60" t="s">
+        <v>384</v>
+      </c>
+      <c r="Q23" s="22" t="s">
+        <v>345</v>
+      </c>
+      <c r="R23" t="s">
+        <v>49</v>
+      </c>
       <c r="S23" s="19" t="s">
         <v>287</v>
       </c>
@@ -6369,7 +6835,7 @@
       <c r="W23" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X23" s="64" t="s">
+      <c r="X23" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y23" s="39" t="s">
@@ -6378,27 +6844,27 @@
       <c r="Z23" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA23" s="64" t="s">
+      <c r="AA23" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB23" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC23" s="63" t="s">
+      <c r="AC23" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD23" s="63" t="s">
+      <c r="AD23" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE23" s="63" t="s">
+      <c r="AE23" s="62" t="s">
         <v>263</v>
       </c>
-      <c r="AF23" s="63" t="s">
+      <c r="AF23" s="62" t="s">
         <v>247</v>
       </c>
       <c r="AG23" s="18"/>
       <c r="AH23" s="4"/>
-      <c r="AI23" s="63">
+      <c r="AI23" s="62">
         <v>4.9535613734183368</v>
       </c>
       <c r="AJ23" s="15"/>
@@ -6447,16 +6913,16 @@
       <c r="AZ23">
         <v>300</v>
       </c>
-      <c r="BB23" s="65" t="s">
+      <c r="BB23" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC23" s="65" t="s">
+      <c r="BC23" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD23" s="65" t="s">
+      <c r="BD23" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE23" s="65" t="s">
+      <c r="BE23" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG23" s="28">
@@ -6490,7 +6956,7 @@
     </row>
     <row r="24" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A24" s="14">
-        <f>COUNTIF(D24,"&lt;&gt;"&amp;"")+COUNTIF(BL24,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B24" s="26">
@@ -6526,10 +6992,21 @@
       <c r="M24" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N24" s="43"/>
-      <c r="O24" s="46"/>
-      <c r="P24" s="60"/>
-      <c r="Q24" s="22"/>
+      <c r="N24" s="43">
+        <v>200109</v>
+      </c>
+      <c r="O24" s="46">
+        <v>200109</v>
+      </c>
+      <c r="P24" s="60" t="s">
+        <v>385</v>
+      </c>
+      <c r="Q24" s="22" t="s">
+        <v>346</v>
+      </c>
+      <c r="R24" t="s">
+        <v>49</v>
+      </c>
       <c r="S24" s="19" t="s">
         <v>288</v>
       </c>
@@ -6543,7 +7020,7 @@
       <c r="W24" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X24" s="64" t="s">
+      <c r="X24" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y24" s="39" t="s">
@@ -6552,27 +7029,27 @@
       <c r="Z24" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA24" s="64" t="s">
+      <c r="AA24" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB24" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC24" s="63" t="s">
+      <c r="AC24" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD24" s="63" t="s">
+      <c r="AD24" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE24" s="63" t="s">
+      <c r="AE24" s="62" t="s">
         <v>264</v>
       </c>
-      <c r="AF24" s="63" t="s">
+      <c r="AF24" s="62" t="s">
         <v>248</v>
       </c>
       <c r="AG24" s="18"/>
       <c r="AH24" s="4"/>
-      <c r="AI24" s="63">
+      <c r="AI24" s="62">
         <v>3.3484353257176145</v>
       </c>
       <c r="AJ24" s="15"/>
@@ -6621,16 +7098,16 @@
       <c r="AZ24">
         <v>300</v>
       </c>
-      <c r="BB24" s="65" t="s">
+      <c r="BB24" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC24" s="65" t="s">
+      <c r="BC24" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD24" s="65" t="s">
+      <c r="BD24" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE24" s="65" t="s">
+      <c r="BE24" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG24" s="28">
@@ -6664,7 +7141,7 @@
     </row>
     <row r="25" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A25" s="14">
-        <f>COUNTIF(D25,"&lt;&gt;"&amp;"")+COUNTIF(BL25,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B25" s="26">
@@ -6700,10 +7177,21 @@
       <c r="M25" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N25" s="43"/>
-      <c r="O25" s="46"/>
-      <c r="P25" s="60"/>
-      <c r="Q25" s="22"/>
+      <c r="N25" s="43">
+        <v>192881</v>
+      </c>
+      <c r="O25" s="46">
+        <v>192881</v>
+      </c>
+      <c r="P25" s="60" t="s">
+        <v>386</v>
+      </c>
+      <c r="Q25" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="R25" t="s">
+        <v>49</v>
+      </c>
       <c r="S25" s="19" t="s">
         <v>289</v>
       </c>
@@ -6717,7 +7205,7 @@
       <c r="W25" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X25" s="64" t="s">
+      <c r="X25" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y25" s="39" t="s">
@@ -6726,27 +7214,27 @@
       <c r="Z25" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA25" s="64" t="s">
+      <c r="AA25" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB25" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC25" s="63" t="s">
+      <c r="AC25" s="62" t="s">
         <v>252</v>
       </c>
-      <c r="AD25" s="63" t="s">
+      <c r="AD25" s="62" t="s">
         <v>236</v>
       </c>
-      <c r="AE25" s="63" t="s">
+      <c r="AE25" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="AF25" s="63" t="s">
+      <c r="AF25" s="62" t="s">
         <v>249</v>
       </c>
       <c r="AG25" s="18"/>
       <c r="AH25" s="4"/>
-      <c r="AI25" s="63">
+      <c r="AI25" s="62">
         <v>2.2605525171785161</v>
       </c>
       <c r="AJ25" s="15"/>
@@ -6795,16 +7283,16 @@
       <c r="AZ25">
         <v>300</v>
       </c>
-      <c r="BB25" s="65" t="s">
+      <c r="BB25" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC25" s="65" t="s">
+      <c r="BC25" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD25" s="65" t="s">
+      <c r="BD25" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE25" s="65" t="s">
+      <c r="BE25" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG25" s="28">
@@ -6838,7 +7326,7 @@
     </row>
     <row r="26" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A26" s="14">
-        <f>COUNTIF(D26,"&lt;&gt;"&amp;"")+COUNTIF(BL26,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B26" s="26">
@@ -6874,10 +7362,21 @@
       <c r="M26" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N26" s="43"/>
-      <c r="O26" s="46"/>
-      <c r="P26" s="60"/>
-      <c r="Q26" s="22"/>
+      <c r="N26" s="43">
+        <v>149812</v>
+      </c>
+      <c r="O26" s="46">
+        <v>149812</v>
+      </c>
+      <c r="P26" s="60" t="s">
+        <v>387</v>
+      </c>
+      <c r="Q26" s="22" t="s">
+        <v>348</v>
+      </c>
+      <c r="R26" t="s">
+        <v>49</v>
+      </c>
       <c r="S26" s="19" t="s">
         <v>290</v>
       </c>
@@ -6891,7 +7390,7 @@
       <c r="W26" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X26" s="64" t="s">
+      <c r="X26" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y26" s="39" t="s">
@@ -6900,27 +7399,27 @@
       <c r="Z26" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA26" s="64" t="s">
+      <c r="AA26" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB26" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC26" s="63" t="s">
+      <c r="AC26" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD26" s="63" t="s">
+      <c r="AD26" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE26" s="63" t="s">
+      <c r="AE26" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="AF26" s="63" t="s">
+      <c r="AF26" s="62" t="s">
         <v>250</v>
       </c>
       <c r="AG26" s="18"/>
       <c r="AH26" s="4"/>
-      <c r="AI26" s="63">
+      <c r="AI26" s="62">
         <v>7.3035392597866311</v>
       </c>
       <c r="AJ26" s="15"/>
@@ -6969,16 +7468,16 @@
       <c r="AZ26">
         <v>300</v>
       </c>
-      <c r="BB26" s="65" t="s">
+      <c r="BB26" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC26" s="65" t="s">
+      <c r="BC26" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD26" s="65" t="s">
+      <c r="BD26" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE26" s="65" t="s">
+      <c r="BE26" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG26" s="28">
@@ -7012,7 +7511,7 @@
     </row>
     <row r="27" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A27" s="14">
-        <f>COUNTIF(D27,"&lt;&gt;"&amp;"")+COUNTIF(BL27,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B27" s="26">
@@ -7048,10 +7547,21 @@
       <c r="M27" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N27" s="43"/>
-      <c r="O27" s="46"/>
-      <c r="P27" s="60"/>
-      <c r="Q27" s="22"/>
+      <c r="N27" s="43">
+        <v>121678</v>
+      </c>
+      <c r="O27" s="46">
+        <v>121678</v>
+      </c>
+      <c r="P27" s="60" t="s">
+        <v>388</v>
+      </c>
+      <c r="Q27" s="22" t="s">
+        <v>349</v>
+      </c>
+      <c r="R27" t="s">
+        <v>49</v>
+      </c>
       <c r="S27" s="19" t="s">
         <v>291</v>
       </c>
@@ -7065,7 +7575,7 @@
       <c r="W27" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X27" s="64" t="s">
+      <c r="X27" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y27" s="39" t="s">
@@ -7074,27 +7584,27 @@
       <c r="Z27" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA27" s="64" t="s">
+      <c r="AA27" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB27" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC27" s="63" t="s">
+      <c r="AC27" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD27" s="63" t="s">
+      <c r="AD27" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE27" s="63" t="s">
+      <c r="AE27" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="AF27" s="63" t="s">
+      <c r="AF27" s="62" t="s">
         <v>239</v>
       </c>
       <c r="AG27" s="18"/>
       <c r="AH27" s="4"/>
-      <c r="AI27" s="63">
+      <c r="AI27" s="62">
         <v>1.7233530737948071</v>
       </c>
       <c r="AJ27" s="15"/>
@@ -7143,16 +7653,16 @@
       <c r="AZ27">
         <v>300</v>
       </c>
-      <c r="BB27" s="65" t="s">
+      <c r="BB27" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC27" s="65" t="s">
+      <c r="BC27" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD27" s="65" t="s">
+      <c r="BD27" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE27" s="65" t="s">
+      <c r="BE27" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG27" s="28">
@@ -7184,7 +7694,7 @@
     </row>
     <row r="28" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A28" s="14">
-        <f>COUNTIF(D28,"&lt;&gt;"&amp;"")+COUNTIF(BL28,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B28" s="26">
@@ -7220,10 +7730,21 @@
       <c r="M28" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N28" s="43"/>
-      <c r="O28" s="46"/>
-      <c r="P28" s="60"/>
-      <c r="Q28" s="22"/>
+      <c r="N28" s="43">
+        <v>324624</v>
+      </c>
+      <c r="O28" s="46">
+        <v>324624</v>
+      </c>
+      <c r="P28" s="60" t="s">
+        <v>389</v>
+      </c>
+      <c r="Q28" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="R28" t="s">
+        <v>49</v>
+      </c>
       <c r="S28" s="19" t="s">
         <v>292</v>
       </c>
@@ -7237,7 +7758,7 @@
       <c r="W28" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X28" s="64" t="s">
+      <c r="X28" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y28" s="39" t="s">
@@ -7246,27 +7767,27 @@
       <c r="Z28" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA28" s="64" t="s">
+      <c r="AA28" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB28" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC28" s="63" t="s">
+      <c r="AC28" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD28" s="63" t="s">
+      <c r="AD28" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE28" s="63" t="s">
+      <c r="AE28" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="AF28" s="63" t="s">
+      <c r="AF28" s="62" t="s">
         <v>240</v>
       </c>
       <c r="AG28" s="18"/>
       <c r="AH28" s="4"/>
-      <c r="AI28" s="63">
+      <c r="AI28" s="62">
         <v>2.1834244846445099</v>
       </c>
       <c r="AJ28" s="15"/>
@@ -7315,16 +7836,16 @@
       <c r="AZ28">
         <v>300</v>
       </c>
-      <c r="BB28" s="65" t="s">
+      <c r="BB28" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC28" s="65" t="s">
+      <c r="BC28" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD28" s="65" t="s">
+      <c r="BD28" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE28" s="65" t="s">
+      <c r="BE28" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG28" s="28">
@@ -7356,7 +7877,7 @@
     </row>
     <row r="29" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A29" s="14">
-        <f>COUNTIF(D29,"&lt;&gt;"&amp;"")+COUNTIF(BL29,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B29" s="26">
@@ -7392,10 +7913,21 @@
       <c r="M29" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N29" s="43"/>
-      <c r="O29" s="46"/>
-      <c r="P29" s="60"/>
-      <c r="Q29" s="22"/>
+      <c r="N29" s="43">
+        <v>135918</v>
+      </c>
+      <c r="O29" s="46">
+        <v>135918</v>
+      </c>
+      <c r="P29" s="60" t="s">
+        <v>390</v>
+      </c>
+      <c r="Q29" s="22" t="s">
+        <v>351</v>
+      </c>
+      <c r="R29" t="s">
+        <v>49</v>
+      </c>
       <c r="S29" s="19" t="s">
         <v>293</v>
       </c>
@@ -7409,7 +7941,7 @@
       <c r="W29" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X29" s="64" t="s">
+      <c r="X29" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y29" s="39" t="s">
@@ -7418,27 +7950,27 @@
       <c r="Z29" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA29" s="64" t="s">
+      <c r="AA29" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB29" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC29" s="63" t="s">
+      <c r="AC29" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD29" s="63" t="s">
+      <c r="AD29" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE29" s="63" t="s">
+      <c r="AE29" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="AF29" s="63" t="s">
+      <c r="AF29" s="62" t="s">
         <v>241</v>
       </c>
       <c r="AG29" s="18"/>
       <c r="AH29" s="4"/>
-      <c r="AI29" s="63">
+      <c r="AI29" s="62">
         <v>2.8624747850662868</v>
       </c>
       <c r="AJ29" s="15"/>
@@ -7487,16 +8019,16 @@
       <c r="AZ29">
         <v>300</v>
       </c>
-      <c r="BB29" s="65" t="s">
+      <c r="BB29" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC29" s="65" t="s">
+      <c r="BC29" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD29" s="65" t="s">
+      <c r="BD29" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE29" s="65" t="s">
+      <c r="BE29" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG29" s="28">
@@ -7528,7 +8060,7 @@
     </row>
     <row r="30" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A30" s="14">
-        <f>COUNTIF(D30,"&lt;&gt;"&amp;"")+COUNTIF(BL30,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B30" s="26">
@@ -7564,10 +8096,21 @@
       <c r="M30" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N30" s="43"/>
-      <c r="O30" s="46"/>
-      <c r="P30" s="60"/>
-      <c r="Q30" s="22"/>
+      <c r="N30" s="43">
+        <v>193005</v>
+      </c>
+      <c r="O30" s="46">
+        <v>193005</v>
+      </c>
+      <c r="P30" s="60" t="s">
+        <v>391</v>
+      </c>
+      <c r="Q30" s="22" t="s">
+        <v>352</v>
+      </c>
+      <c r="R30" t="s">
+        <v>49</v>
+      </c>
       <c r="S30" s="19" t="s">
         <v>294</v>
       </c>
@@ -7581,7 +8124,7 @@
       <c r="W30" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X30" s="64" t="s">
+      <c r="X30" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y30" s="39" t="s">
@@ -7590,27 +8133,27 @@
       <c r="Z30" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA30" s="64" t="s">
+      <c r="AA30" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC30" s="63" t="s">
+      <c r="AC30" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD30" s="63" t="s">
+      <c r="AD30" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE30" s="63" t="s">
+      <c r="AE30" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="AF30" s="63" t="s">
+      <c r="AF30" s="62" t="s">
         <v>242</v>
       </c>
       <c r="AG30" s="18"/>
       <c r="AH30" s="4"/>
-      <c r="AI30" s="63">
+      <c r="AI30" s="62">
         <v>6.1493155561308699</v>
       </c>
       <c r="AJ30" s="15"/>
@@ -7659,16 +8202,16 @@
       <c r="AZ30">
         <v>300</v>
       </c>
-      <c r="BB30" s="65" t="s">
+      <c r="BB30" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC30" s="65" t="s">
+      <c r="BC30" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD30" s="65" t="s">
+      <c r="BD30" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE30" s="65" t="s">
+      <c r="BE30" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG30" s="28">
@@ -7700,7 +8243,7 @@
     </row>
     <row r="31" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A31" s="14">
-        <f>COUNTIF(D31,"&lt;&gt;"&amp;"")+COUNTIF(BL31,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B31" s="26">
@@ -7736,10 +8279,21 @@
       <c r="M31" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N31" s="43"/>
-      <c r="O31" s="46"/>
-      <c r="P31" s="60"/>
-      <c r="Q31" s="22"/>
+      <c r="N31" s="43">
+        <v>165278</v>
+      </c>
+      <c r="O31" s="46">
+        <v>165278</v>
+      </c>
+      <c r="P31" s="60" t="s">
+        <v>392</v>
+      </c>
+      <c r="Q31" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="R31" t="s">
+        <v>49</v>
+      </c>
       <c r="S31" s="19" t="s">
         <v>295</v>
       </c>
@@ -7753,7 +8307,7 @@
       <c r="W31" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X31" s="64" t="s">
+      <c r="X31" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y31" s="39" t="s">
@@ -7762,27 +8316,27 @@
       <c r="Z31" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA31" s="64" t="s">
+      <c r="AA31" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB31" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC31" s="63" t="s">
+      <c r="AC31" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD31" s="63" t="s">
+      <c r="AD31" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE31" s="63" t="s">
+      <c r="AE31" s="62" t="s">
         <v>259</v>
       </c>
-      <c r="AF31" s="63" t="s">
+      <c r="AF31" s="62" t="s">
         <v>243</v>
       </c>
       <c r="AG31" s="18"/>
       <c r="AH31" s="4"/>
-      <c r="AI31" s="63">
+      <c r="AI31" s="62">
         <v>11.453890381109566</v>
       </c>
       <c r="AJ31" s="15"/>
@@ -7831,16 +8385,16 @@
       <c r="AZ31">
         <v>300</v>
       </c>
-      <c r="BB31" s="65" t="s">
+      <c r="BB31" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC31" s="65" t="s">
+      <c r="BC31" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD31" s="65" t="s">
+      <c r="BD31" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE31" s="65" t="s">
+      <c r="BE31" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG31" s="28">
@@ -7872,7 +8426,7 @@
     </row>
     <row r="32" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A32" s="14">
-        <f>COUNTIF(D32,"&lt;&gt;"&amp;"")+COUNTIF(BL32,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B32" s="26">
@@ -7908,10 +8462,21 @@
       <c r="M32" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N32" s="43"/>
-      <c r="O32" s="46"/>
-      <c r="P32" s="60"/>
-      <c r="Q32" s="22"/>
+      <c r="N32" s="43">
+        <v>63186</v>
+      </c>
+      <c r="O32" s="46">
+        <v>63186</v>
+      </c>
+      <c r="P32" s="60" t="s">
+        <v>393</v>
+      </c>
+      <c r="Q32" s="22" t="s">
+        <v>354</v>
+      </c>
+      <c r="R32" t="s">
+        <v>49</v>
+      </c>
       <c r="S32" s="19" t="s">
         <v>296</v>
       </c>
@@ -7925,7 +8490,7 @@
       <c r="W32" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X32" s="64" t="s">
+      <c r="X32" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y32" s="39" t="s">
@@ -7934,27 +8499,27 @@
       <c r="Z32" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA32" s="64" t="s">
+      <c r="AA32" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB32" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC32" s="63" t="s">
+      <c r="AC32" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD32" s="63" t="s">
+      <c r="AD32" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE32" s="63" t="s">
+      <c r="AE32" s="62" t="s">
         <v>260</v>
       </c>
-      <c r="AF32" s="63" t="s">
+      <c r="AF32" s="62" t="s">
         <v>244</v>
       </c>
       <c r="AG32" s="18"/>
       <c r="AH32" s="4"/>
-      <c r="AI32" s="63">
+      <c r="AI32" s="62">
         <v>4.5420320809466794</v>
       </c>
       <c r="AJ32" s="15"/>
@@ -8003,16 +8568,16 @@
       <c r="AZ32">
         <v>300</v>
       </c>
-      <c r="BB32" s="65" t="s">
+      <c r="BB32" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC32" s="65" t="s">
+      <c r="BC32" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD32" s="65" t="s">
+      <c r="BD32" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE32" s="65" t="s">
+      <c r="BE32" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG32" s="28">
@@ -8044,7 +8609,7 @@
     </row>
     <row r="33" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A33" s="14">
-        <f>COUNTIF(D33,"&lt;&gt;"&amp;"")+COUNTIF(BL33,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B33" s="26">
@@ -8080,10 +8645,21 @@
       <c r="M33" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N33" s="43"/>
-      <c r="O33" s="46"/>
-      <c r="P33" s="60"/>
-      <c r="Q33" s="22"/>
+      <c r="N33" s="43">
+        <v>145904</v>
+      </c>
+      <c r="O33" s="46">
+        <v>145904</v>
+      </c>
+      <c r="P33" s="60" t="s">
+        <v>394</v>
+      </c>
+      <c r="Q33" s="22" t="s">
+        <v>355</v>
+      </c>
+      <c r="R33" t="s">
+        <v>49</v>
+      </c>
       <c r="S33" s="19" t="s">
         <v>297</v>
       </c>
@@ -8097,7 +8673,7 @@
       <c r="W33" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X33" s="64" t="s">
+      <c r="X33" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y33" s="39" t="s">
@@ -8106,27 +8682,27 @@
       <c r="Z33" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA33" s="64" t="s">
+      <c r="AA33" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB33" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC33" s="63" t="s">
+      <c r="AC33" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD33" s="63" t="s">
+      <c r="AD33" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE33" s="63" t="s">
+      <c r="AE33" s="62" t="s">
         <v>261</v>
       </c>
-      <c r="AF33" s="63" t="s">
+      <c r="AF33" s="62" t="s">
         <v>245</v>
       </c>
       <c r="AG33" s="18"/>
       <c r="AH33" s="4"/>
-      <c r="AI33" s="63">
+      <c r="AI33" s="62">
         <v>4.059847038391422</v>
       </c>
       <c r="AJ33" s="15"/>
@@ -8175,16 +8751,16 @@
       <c r="AZ33">
         <v>300</v>
       </c>
-      <c r="BB33" s="65" t="s">
+      <c r="BB33" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC33" s="65" t="s">
+      <c r="BC33" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD33" s="65" t="s">
+      <c r="BD33" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE33" s="65" t="s">
+      <c r="BE33" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG33" s="28">
@@ -8216,7 +8792,7 @@
     </row>
     <row r="34" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A34" s="14">
-        <f>COUNTIF(D34,"&lt;&gt;"&amp;"")+COUNTIF(BL34,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" si="0"/>
         <v>1</v>
       </c>
       <c r="B34" s="26">
@@ -8252,10 +8828,21 @@
       <c r="M34" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="N34" s="43"/>
-      <c r="O34" s="46"/>
-      <c r="P34" s="61"/>
-      <c r="Q34" s="22"/>
+      <c r="N34" s="43">
+        <v>133913</v>
+      </c>
+      <c r="O34" s="46">
+        <v>133913</v>
+      </c>
+      <c r="P34" s="61" t="s">
+        <v>395</v>
+      </c>
+      <c r="Q34" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="R34" t="s">
+        <v>49</v>
+      </c>
       <c r="S34" s="19" t="s">
         <v>298</v>
       </c>
@@ -8269,7 +8856,7 @@
       <c r="W34" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X34" s="64" t="s">
+      <c r="X34" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y34" s="39" t="s">
@@ -8278,27 +8865,27 @@
       <c r="Z34" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA34" s="64" t="s">
+      <c r="AA34" s="63" t="s">
         <v>311</v>
       </c>
       <c r="AB34" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="AC34" s="63" t="s">
+      <c r="AC34" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD34" s="63" t="s">
+      <c r="AD34" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE34" s="63" t="s">
+      <c r="AE34" s="62" t="s">
         <v>262</v>
       </c>
-      <c r="AF34" s="63" t="s">
+      <c r="AF34" s="62" t="s">
         <v>246</v>
       </c>
       <c r="AG34" s="18"/>
       <c r="AH34" s="4"/>
-      <c r="AI34" s="63">
+      <c r="AI34" s="62">
         <v>3.7195128528742329</v>
       </c>
       <c r="AJ34" s="15"/>
@@ -8347,16 +8934,16 @@
       <c r="AZ34">
         <v>300</v>
       </c>
-      <c r="BB34" s="65" t="s">
+      <c r="BB34" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC34" s="65" t="s">
+      <c r="BC34" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD34" s="65" t="s">
+      <c r="BD34" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE34" s="65" t="s">
+      <c r="BE34" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG34" s="28">
@@ -8388,7 +8975,7 @@
     </row>
     <row r="35" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A35" s="14">
-        <f t="shared" ref="A35:A41" si="0">COUNTIF(D35,"&lt;&gt;"&amp;"")+COUNTIF(BL35,"&lt;&gt;"&amp;"")</f>
+        <f t="shared" ref="A35:A41" si="1">COUNTIF(D35,"&lt;&gt;"&amp;"")+COUNTIF(BL35,"&lt;&gt;"&amp;"")</f>
         <v>1</v>
       </c>
       <c r="B35" s="26">
@@ -8425,7 +9012,21 @@
       <c r="M35" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="P35" s="2"/>
+      <c r="N35" s="44">
+        <v>262994</v>
+      </c>
+      <c r="O35" s="47">
+        <v>262994</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>396</v>
+      </c>
+      <c r="Q35" s="67" t="s">
+        <v>357</v>
+      </c>
+      <c r="R35" t="s">
+        <v>49</v>
+      </c>
       <c r="S35" t="s">
         <v>299</v>
       </c>
@@ -8438,7 +9039,7 @@
       <c r="W35" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X35" s="64" t="s">
+      <c r="X35" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y35" s="39" t="s">
@@ -8447,23 +9048,23 @@
       <c r="Z35" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA35" s="64" t="s">
+      <c r="AA35" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC35" s="63" t="s">
+      <c r="AC35" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD35" s="63" t="s">
+      <c r="AD35" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE35" s="63" t="s">
+      <c r="AE35" s="62" t="s">
         <v>264</v>
       </c>
-      <c r="AF35" s="63" t="s">
+      <c r="AF35" s="62" t="s">
         <v>248</v>
       </c>
       <c r="AG35"/>
-      <c r="AI35" s="63">
+      <c r="AI35" s="62">
         <v>1.0464602008564987</v>
       </c>
       <c r="AJ35" s="15"/>
@@ -8509,16 +9110,16 @@
       <c r="AZ35">
         <v>300</v>
       </c>
-      <c r="BB35" s="65" t="s">
+      <c r="BB35" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC35" s="65" t="s">
+      <c r="BC35" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD35" s="65" t="s">
+      <c r="BD35" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE35" s="65" t="s">
+      <c r="BE35" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG35" s="28">
@@ -8552,7 +9153,7 @@
     </row>
     <row r="36" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A36" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B36" s="26">
@@ -8588,7 +9189,21 @@
       <c r="M36" s="36" t="s">
         <v>49</v>
       </c>
-      <c r="P36" s="2"/>
+      <c r="N36" s="44">
+        <v>265152</v>
+      </c>
+      <c r="O36" s="47">
+        <v>265152</v>
+      </c>
+      <c r="P36" s="2" t="s">
+        <v>397</v>
+      </c>
+      <c r="Q36" t="s">
+        <v>358</v>
+      </c>
+      <c r="R36" t="s">
+        <v>49</v>
+      </c>
       <c r="S36" s="19" t="s">
         <v>300</v>
       </c>
@@ -8601,7 +9216,7 @@
       <c r="W36" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X36" s="64" t="s">
+      <c r="X36" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y36" s="39" t="s">
@@ -8610,22 +9225,22 @@
       <c r="Z36" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA36" s="64" t="s">
+      <c r="AA36" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC36" s="63" t="s">
+      <c r="AC36" s="62" t="s">
         <v>253</v>
       </c>
-      <c r="AD36" s="63" t="s">
+      <c r="AD36" s="62" t="s">
         <v>237</v>
       </c>
-      <c r="AE36" s="63" t="s">
+      <c r="AE36" s="62" t="s">
         <v>265</v>
       </c>
-      <c r="AF36" s="63" t="s">
+      <c r="AF36" s="62" t="s">
         <v>249</v>
       </c>
-      <c r="AI36" s="63">
+      <c r="AI36" s="62">
         <v>2.932051821408153</v>
       </c>
       <c r="AJ36" s="15"/>
@@ -8671,16 +9286,16 @@
       <c r="AZ36">
         <v>300</v>
       </c>
-      <c r="BB36" s="65" t="s">
+      <c r="BB36" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC36" s="65" t="s">
+      <c r="BC36" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD36" s="65" t="s">
+      <c r="BD36" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE36" s="65" t="s">
+      <c r="BE36" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG36" s="28">
@@ -8707,7 +9322,7 @@
     </row>
     <row r="37" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A37" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B37" s="26">
@@ -8743,6 +9358,21 @@
       <c r="M37" s="36" t="s">
         <v>49</v>
       </c>
+      <c r="N37" s="44">
+        <v>221716</v>
+      </c>
+      <c r="O37" s="47">
+        <v>221716</v>
+      </c>
+      <c r="P37" t="s">
+        <v>398</v>
+      </c>
+      <c r="Q37" t="s">
+        <v>359</v>
+      </c>
+      <c r="R37" t="s">
+        <v>49</v>
+      </c>
       <c r="S37" s="19" t="s">
         <v>301</v>
       </c>
@@ -8755,7 +9385,7 @@
       <c r="W37" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X37" s="64" t="s">
+      <c r="X37" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y37" s="39" t="s">
@@ -8764,22 +9394,22 @@
       <c r="Z37" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA37" s="64" t="s">
+      <c r="AA37" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC37" s="63" t="s">
+      <c r="AC37" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="AD37" s="63" t="s">
+      <c r="AD37" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="AE37" s="63" t="s">
+      <c r="AE37" s="62" t="s">
         <v>266</v>
       </c>
-      <c r="AF37" s="63" t="s">
+      <c r="AF37" s="62" t="s">
         <v>250</v>
       </c>
-      <c r="AI37" s="63">
+      <c r="AI37" s="62">
         <v>0.63924576335177929</v>
       </c>
       <c r="AJ37" s="15"/>
@@ -8825,16 +9455,16 @@
       <c r="AZ37">
         <v>300</v>
       </c>
-      <c r="BB37" s="65" t="s">
+      <c r="BB37" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC37" s="65" t="s">
+      <c r="BC37" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD37" s="65" t="s">
+      <c r="BD37" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE37" s="65" t="s">
+      <c r="BE37" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG37" s="28">
@@ -8861,7 +9491,7 @@
     </row>
     <row r="38" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A38" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B38" s="26">
@@ -8897,6 +9527,21 @@
       <c r="M38" s="36" t="s">
         <v>49</v>
       </c>
+      <c r="N38" s="44">
+        <v>162989</v>
+      </c>
+      <c r="O38" s="47">
+        <v>162989</v>
+      </c>
+      <c r="P38" t="s">
+        <v>399</v>
+      </c>
+      <c r="Q38" t="s">
+        <v>360</v>
+      </c>
+      <c r="R38" t="s">
+        <v>49</v>
+      </c>
       <c r="S38" s="19" t="s">
         <v>302</v>
       </c>
@@ -8909,7 +9554,7 @@
       <c r="W38" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X38" s="64" t="s">
+      <c r="X38" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y38" s="39" t="s">
@@ -8918,22 +9563,22 @@
       <c r="Z38" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA38" s="64" t="s">
+      <c r="AA38" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC38" s="63" t="s">
+      <c r="AC38" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="AD38" s="63" t="s">
+      <c r="AD38" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="AE38" s="63" t="s">
+      <c r="AE38" s="62" t="s">
         <v>255</v>
       </c>
-      <c r="AF38" s="63" t="s">
+      <c r="AF38" s="62" t="s">
         <v>239</v>
       </c>
-      <c r="AI38" s="63">
+      <c r="AI38" s="62">
         <v>1.6964168682451353</v>
       </c>
       <c r="AJ38" s="15"/>
@@ -8979,16 +9624,16 @@
       <c r="AZ38">
         <v>300</v>
       </c>
-      <c r="BB38" s="65" t="s">
+      <c r="BB38" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC38" s="65" t="s">
+      <c r="BC38" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD38" s="65" t="s">
+      <c r="BD38" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE38" s="65" t="s">
+      <c r="BE38" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG38" s="28">
@@ -9015,7 +9660,7 @@
     </row>
     <row r="39" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A39" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B39" s="26">
@@ -9051,6 +9696,21 @@
       <c r="M39" s="36" t="s">
         <v>49</v>
       </c>
+      <c r="N39" s="44">
+        <v>178894</v>
+      </c>
+      <c r="O39" s="47">
+        <v>178894</v>
+      </c>
+      <c r="P39" t="s">
+        <v>400</v>
+      </c>
+      <c r="Q39" t="s">
+        <v>361</v>
+      </c>
+      <c r="R39" t="s">
+        <v>49</v>
+      </c>
       <c r="S39" s="19" t="s">
         <v>303</v>
       </c>
@@ -9063,7 +9723,7 @@
       <c r="W39" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X39" s="64" t="s">
+      <c r="X39" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y39" s="39" t="s">
@@ -9072,22 +9732,22 @@
       <c r="Z39" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA39" s="64" t="s">
+      <c r="AA39" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC39" s="63" t="s">
+      <c r="AC39" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="AD39" s="63" t="s">
+      <c r="AD39" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="AE39" s="63" t="s">
+      <c r="AE39" s="62" t="s">
         <v>256</v>
       </c>
-      <c r="AF39" s="63" t="s">
+      <c r="AF39" s="62" t="s">
         <v>240</v>
       </c>
-      <c r="AI39" s="63">
+      <c r="AI39" s="62">
         <v>1.8468657972233908</v>
       </c>
       <c r="AJ39" s="15"/>
@@ -9133,16 +9793,16 @@
       <c r="AZ39">
         <v>300</v>
       </c>
-      <c r="BB39" s="65" t="s">
+      <c r="BB39" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC39" s="65" t="s">
+      <c r="BC39" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD39" s="65" t="s">
+      <c r="BD39" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE39" s="65" t="s">
+      <c r="BE39" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG39" s="28">
@@ -9169,7 +9829,7 @@
     </row>
     <row r="40" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A40" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B40" s="26">
@@ -9205,6 +9865,21 @@
       <c r="M40" s="36" t="s">
         <v>49</v>
       </c>
+      <c r="N40" s="44">
+        <v>229841</v>
+      </c>
+      <c r="O40" s="47">
+        <v>229841</v>
+      </c>
+      <c r="P40" t="s">
+        <v>401</v>
+      </c>
+      <c r="Q40" t="s">
+        <v>362</v>
+      </c>
+      <c r="R40" t="s">
+        <v>49</v>
+      </c>
       <c r="S40" s="19" t="s">
         <v>304</v>
       </c>
@@ -9217,7 +9892,7 @@
       <c r="W40" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X40" s="64" t="s">
+      <c r="X40" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y40" s="39" t="s">
@@ -9226,22 +9901,22 @@
       <c r="Z40" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA40" s="64" t="s">
+      <c r="AA40" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC40" s="63" t="s">
+      <c r="AC40" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="AD40" s="63" t="s">
+      <c r="AD40" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="AE40" s="63" t="s">
+      <c r="AE40" s="62" t="s">
         <v>257</v>
       </c>
-      <c r="AF40" s="63" t="s">
+      <c r="AF40" s="62" t="s">
         <v>241</v>
       </c>
-      <c r="AI40" s="63">
+      <c r="AI40" s="62">
         <v>2.4691674312746512</v>
       </c>
       <c r="AJ40" s="15"/>
@@ -9287,16 +9962,16 @@
       <c r="AZ40">
         <v>300</v>
       </c>
-      <c r="BB40" s="65" t="s">
+      <c r="BB40" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC40" s="65" t="s">
+      <c r="BC40" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD40" s="65" t="s">
+      <c r="BD40" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE40" s="65" t="s">
+      <c r="BE40" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG40" s="28">
@@ -9323,7 +9998,7 @@
     </row>
     <row r="41" spans="1:76" x14ac:dyDescent="0.2">
       <c r="A41" s="14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
       <c r="B41" s="26">
@@ -9359,6 +10034,21 @@
       <c r="M41" s="36" t="s">
         <v>49</v>
       </c>
+      <c r="N41" s="44">
+        <v>208081</v>
+      </c>
+      <c r="O41" s="47">
+        <v>208081</v>
+      </c>
+      <c r="P41" t="s">
+        <v>402</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>363</v>
+      </c>
+      <c r="R41" t="s">
+        <v>49</v>
+      </c>
       <c r="S41" s="19" t="s">
         <v>305</v>
       </c>
@@ -9371,7 +10061,7 @@
       <c r="W41" s="19" t="s">
         <v>308</v>
       </c>
-      <c r="X41" s="64" t="s">
+      <c r="X41" s="63" t="s">
         <v>309</v>
       </c>
       <c r="Y41" s="39" t="s">
@@ -9380,22 +10070,22 @@
       <c r="Z41" s="19" t="s">
         <v>310</v>
       </c>
-      <c r="AA41" s="64" t="s">
+      <c r="AA41" s="63" t="s">
         <v>311</v>
       </c>
-      <c r="AC41" s="63" t="s">
+      <c r="AC41" s="62" t="s">
         <v>254</v>
       </c>
-      <c r="AD41" s="63" t="s">
+      <c r="AD41" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="AE41" s="63" t="s">
+      <c r="AE41" s="62" t="s">
         <v>258</v>
       </c>
-      <c r="AF41" s="63" t="s">
+      <c r="AF41" s="62" t="s">
         <v>242</v>
       </c>
-      <c r="AI41" s="63">
+      <c r="AI41" s="62">
         <v>1.6624057473868159</v>
       </c>
       <c r="AJ41" s="15"/>
@@ -9441,16 +10131,16 @@
       <c r="AZ41">
         <v>300</v>
       </c>
-      <c r="BB41" s="65" t="s">
+      <c r="BB41" s="64" t="s">
         <v>322</v>
       </c>
-      <c r="BC41" s="65" t="s">
+      <c r="BC41" s="64" t="s">
         <v>319</v>
       </c>
-      <c r="BD41" s="65" t="s">
+      <c r="BD41" s="64" t="s">
         <v>320</v>
       </c>
-      <c r="BE41" s="65" t="s">
+      <c r="BE41" s="64" t="s">
         <v>321</v>
       </c>
       <c r="BG41" s="28">
@@ -9476,9 +10166,15 @@
       </c>
     </row>
     <row r="42" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="R42" t="s">
+        <v>49</v>
+      </c>
       <c r="AJ42" s="15"/>
     </row>
     <row r="43" spans="1:76" x14ac:dyDescent="0.2">
+      <c r="R43" t="s">
+        <v>49</v>
+      </c>
       <c r="AJ43" s="15"/>
     </row>
     <row r="44" spans="1:76" x14ac:dyDescent="0.2">
@@ -9546,9 +10242,19 @@
     </row>
   </sheetData>
   <customSheetViews>
-    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
-      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
+    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
+      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
+      <rowBreaks count="2" manualBreakCount="2">
+        <brk id="1" max="16383" man="1"/>
+        <brk id="325" max="16383" man="1"/>
+      </rowBreaks>
+      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+    </customSheetView>
+    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
+      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
@@ -9566,24 +10272,14 @@
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
-    <customSheetView guid="{CB40A2B6-4618-A74E-89AF-8E1F0A1F3C2E}" topLeftCell="AP1">
-      <pane ySplit="2.03125" topLeftCell="A342" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="BA367" sqref="BA367"/>
+    <customSheetView guid="{31EA8456-A0B1-A842-BBBA-1FCBF1E560D2}" topLeftCell="BD1">
+      <pane ySplit="2" topLeftCell="A273" activePane="bottomLeft" state="frozenSplit"/>
+      <selection pane="bottomLeft" activeCell="BG334" sqref="BG334"/>
       <rowBreaks count="2" manualBreakCount="2">
         <brk id="1" max="16383" man="1"/>
         <brk id="325" max="16383" man="1"/>
       </rowBreaks>
       <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-      <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-    </customSheetView>
-    <customSheetView guid="{06B92370-743D-804F-912C-658BE37B1274}" topLeftCell="X1">
-      <pane ySplit="2" topLeftCell="A314" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="AD344" sqref="AD344"/>
-      <rowBreaks count="2" manualBreakCount="2">
-        <brk id="1" max="16383" man="1"/>
-        <brk id="325" max="16383" man="1"/>
-      </rowBreaks>
-      <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
       <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
     </customSheetView>
   </customSheetViews>

</xml_diff>